<commit_message>
Rearranged the creation of the dcat-ap descriptions. Updated some labels, added the public-identifier presentation.
</commit_message>
<xml_diff>
--- a/excelfiles/Core_Vocabularies_v1.3.xlsx
+++ b/excelfiles/Core_Vocabularies_v1.3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8820" tabRatio="522" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8820" tabRatio="522"/>
   </bookViews>
   <sheets>
     <sheet name="CoreVocabularies" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6860" uniqueCount="1612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6862" uniqueCount="1614">
   <si>
     <t>Term</t>
   </si>
@@ -5336,6 +5336,12 @@
   </si>
   <si>
     <t>Target Identifier</t>
+  </si>
+  <si>
+    <t>publicidentifier</t>
+  </si>
+  <si>
+    <t>http://Address/somewhere</t>
   </si>
 </sst>
 </file>
@@ -18484,11 +18490,11 @@
   </sheetPr>
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18562,6 +18568,9 @@
       </c>
       <c r="H2" s="2" t="s">
         <v>392</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>1613</v>
       </c>
       <c r="K2" s="5"/>
     </row>
@@ -21070,11 +21079,12 @@
     <hyperlink ref="F59" location="String" display="String"/>
     <hyperlink ref="F60" location="String" display="String"/>
     <hyperlink ref="F62" location="String" display="String"/>
+    <hyperlink ref="I2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="36" fitToHeight="0" orientation="landscape"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -21583,8 +21593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L579"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21657,6 +21667,9 @@
       </c>
       <c r="H2" t="s">
         <v>911</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1612</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed the data in the excel file (case sensitive ids). Python code could be updated to remove problem, bt trees and index.html.in would all need to be updated.
</commit_message>
<xml_diff>
--- a/excelfiles/Core_Vocabularies_v1.3.xlsx
+++ b/excelfiles/Core_Vocabularies_v1.3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8820" tabRatio="522"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8820" tabRatio="522" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CoreVocabularies" sheetId="1" r:id="rId1"/>
@@ -18490,7 +18490,7 @@
   </sheetPr>
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -21593,8 +21593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L579"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A397" workbookViewId="0">
+      <selection activeCell="A419" sqref="A419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31555,11 +31555,11 @@
   <sheetPr codeName="Sheet3" filterMode="1"/>
   <dimension ref="A1:H1154"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C784" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="F804" sqref="F804"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31567,7 +31567,7 @@
     <col min="1" max="1" width="38.28515625" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="50.42578125" customWidth="1"/>
+    <col min="4" max="4" width="78" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" customWidth="1"/>
     <col min="6" max="6" width="37.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="201.42578125" style="40" bestFit="1" customWidth="1"/>
@@ -47627,13 +47627,13 @@
       </c>
       <c r="D803" s="10" t="str">
         <f t="shared" si="12"/>
-        <v>KoSIT - XOV / anschrift</v>
+        <v>KoSIT - XOV / Anschrift</v>
       </c>
       <c r="E803" s="11" t="s">
         <v>1109</v>
       </c>
       <c r="F803" s="25" t="s">
-        <v>1134</v>
+        <v>1108</v>
       </c>
       <c r="G803" s="10"/>
       <c r="H803" s="47"/>

</xml_diff>

<commit_message>
Fixed a couple of problems in the excel files - mislabelled rows, etc. Extended the scripts to trap a few of them.
</commit_message>
<xml_diff>
--- a/excelfiles/Core_Vocabularies_v1.3.xlsx
+++ b/excelfiles/Core_Vocabularies_v1.3.xlsx
@@ -31556,10 +31556,10 @@
   <dimension ref="A1:H1154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C784" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1050" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F804" sqref="F804"/>
+      <selection pane="bottomRight" activeCell="D1086" sqref="D1086"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51890,7 +51890,7 @@
         <v>273</v>
       </c>
       <c r="C1041" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="D1041" t="str">
         <f t="shared" si="16"/>
@@ -52612,7 +52612,7 @@
         <v>37</v>
       </c>
       <c r="C1083" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="D1083" t="str">
         <f t="shared" si="16"/>

</xml_diff>

<commit_message>
Outstanding updates for last problems spotted by Bert.
</commit_message>
<xml_diff>
--- a/excelfiles/Core_Vocabularies_v1.3.xlsx
+++ b/excelfiles/Core_Vocabularies_v1.3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8820" tabRatio="522" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8820" tabRatio="522"/>
   </bookViews>
   <sheets>
     <sheet name="CoreVocabularies" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6862" uniqueCount="1614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6861" uniqueCount="1613">
   <si>
     <t>Term</t>
   </si>
@@ -5339,9 +5339,6 @@
   </si>
   <si>
     <t>publicidentifier</t>
-  </si>
-  <si>
-    <t>http://Address/somewhere</t>
   </si>
 </sst>
 </file>
@@ -18490,8 +18487,8 @@
   </sheetPr>
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
@@ -18569,9 +18566,7 @@
       <c r="H2" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="I2" s="42" t="s">
-        <v>1613</v>
-      </c>
+      <c r="I2" s="42"/>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -21079,12 +21074,11 @@
     <hyperlink ref="F59" location="String" display="String"/>
     <hyperlink ref="F60" location="String" display="String"/>
     <hyperlink ref="F62" location="String" display="String"/>
-    <hyperlink ref="I2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="36" fitToHeight="0" orientation="landscape"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -31555,8 +31549,8 @@
   <sheetPr codeName="Sheet3" filterMode="1"/>
   <dimension ref="A1:H1154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1050" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F1050" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D1086" sqref="D1086"/>

</xml_diff>